<commit_message>
updated MCI kit demand for Green patients
</commit_message>
<xml_diff>
--- a/MCI_Tool_Input_Example.xlsx
+++ b/MCI_Tool_Input_Example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikola/pyrecodes_hospitals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBFB841-DAA5-E04B-9B1F-3D4F301A3CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E67C4D19-165B-6449-A64C-1641CFB6742E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{8A19E584-5C10-AD41-83D9-0E8D98A88E8A}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" activeTab="2" xr2:uid="{8A19E584-5C10-AD41-83D9-0E8D98A88E8A}"/>
   </bookViews>
   <sheets>
     <sheet name="ResourceSupply" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1161" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1165" uniqueCount="120">
   <si>
     <t>Nurses</t>
   </si>
@@ -1770,6 +1770,21 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1797,26 +1812,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2150,7 +2150,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="89" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -2198,7 +2198,7 @@
       <c r="G3" s="19"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="161" t="s">
+      <c r="A4" s="166" t="s">
         <v>93</v>
       </c>
       <c r="B4" s="84" t="s">
@@ -2216,7 +2216,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="162"/>
+      <c r="A5" s="167"/>
       <c r="B5" s="87" t="s">
         <v>68</v>
       </c>
@@ -2232,7 +2232,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="162"/>
+      <c r="A6" s="167"/>
       <c r="B6" s="88" t="s">
         <v>67</v>
       </c>
@@ -2248,7 +2248,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="162"/>
+      <c r="A7" s="167"/>
       <c r="B7" s="89" t="s">
         <v>69</v>
       </c>
@@ -2264,7 +2264,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="163"/>
+      <c r="A8" s="168"/>
       <c r="B8" s="90" t="s">
         <v>83</v>
       </c>
@@ -2319,7 +2319,7 @@
       <c r="A12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="164" t="s">
+      <c r="B12" s="169" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="29">
@@ -2336,7 +2336,7 @@
       <c r="A13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="165"/>
+      <c r="B13" s="170"/>
       <c r="C13" s="29">
         <f>30000+100000</f>
         <v>130000</v>
@@ -2353,7 +2353,7 @@
       <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="165"/>
+      <c r="B14" s="170"/>
       <c r="C14" s="30">
         <v>8</v>
       </c>
@@ -2365,7 +2365,7 @@
       <c r="A15" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="166"/>
+      <c r="B15" s="171"/>
       <c r="C15" s="29">
         <v>12000</v>
       </c>
@@ -2386,7 +2386,7 @@
       <c r="A18" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="167" t="s">
+      <c r="B18" s="172" t="s">
         <v>1</v>
       </c>
       <c r="C18" s="102">
@@ -2400,7 +2400,7 @@
       <c r="A19" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="168"/>
+      <c r="B19" s="173"/>
       <c r="C19" s="31">
         <v>5000000</v>
       </c>
@@ -2412,7 +2412,7 @@
       <c r="A20" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="168"/>
+      <c r="B20" s="173"/>
       <c r="C20" s="102">
         <v>24</v>
       </c>
@@ -2424,7 +2424,7 @@
       <c r="A21" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="169"/>
+      <c r="B21" s="174"/>
       <c r="C21" s="31">
         <v>500000</v>
       </c>
@@ -2448,7 +2448,7 @@
       <c r="A24" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="167" t="s">
+      <c r="B24" s="172" t="s">
         <v>1</v>
       </c>
       <c r="C24" s="31">
@@ -2462,7 +2462,7 @@
       <c r="A25" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B25" s="168"/>
+      <c r="B25" s="173"/>
       <c r="C25" s="31">
         <v>200000</v>
       </c>
@@ -2474,7 +2474,7 @@
       <c r="A26" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="168"/>
+      <c r="B26" s="173"/>
       <c r="C26" s="31">
         <v>0</v>
       </c>
@@ -2486,7 +2486,7 @@
       <c r="A27" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="169"/>
+      <c r="B27" s="174"/>
       <c r="C27" s="31">
         <v>0</v>
       </c>
@@ -2506,7 +2506,7 @@
       <c r="F29" s="6"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="171" t="s">
+      <c r="A30" s="175" t="s">
         <v>71</v>
       </c>
       <c r="B30" s="85" t="s">
@@ -2522,7 +2522,7 @@
       <c r="F30" s="6"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="172"/>
+      <c r="A31" s="176"/>
       <c r="B31" s="96" t="s">
         <v>68</v>
       </c>
@@ -2536,7 +2536,7 @@
       <c r="F31" s="6"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="172"/>
+      <c r="A32" s="176"/>
       <c r="B32" s="96" t="s">
         <v>67</v>
       </c>
@@ -2550,7 +2550,7 @@
       <c r="F32" s="6"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="172"/>
+      <c r="A33" s="176"/>
       <c r="B33" s="89" t="s">
         <v>69</v>
       </c>
@@ -2567,7 +2567,7 @@
       <c r="A34" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B34" s="170" t="s">
+      <c r="B34" s="162" t="s">
         <v>1</v>
       </c>
       <c r="C34" s="29">
@@ -2583,7 +2583,7 @@
       <c r="A35" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B35" s="170"/>
+      <c r="B35" s="162"/>
       <c r="C35" s="29">
         <v>72</v>
       </c>
@@ -2597,7 +2597,7 @@
       <c r="A36" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B36" s="170"/>
+      <c r="B36" s="162"/>
       <c r="C36" s="29">
         <v>0</v>
       </c>
@@ -2611,7 +2611,7 @@
       <c r="A37" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B37" s="170"/>
+      <c r="B37" s="162"/>
       <c r="C37" s="29">
         <v>0</v>
       </c>
@@ -2639,7 +2639,7 @@
       <c r="A40" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="B40" s="170" t="s">
+      <c r="B40" s="162" t="s">
         <v>1</v>
       </c>
       <c r="C40" s="102">
@@ -2653,7 +2653,7 @@
       <c r="A41" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="B41" s="170"/>
+      <c r="B41" s="162"/>
       <c r="C41" s="31">
         <v>6</v>
       </c>
@@ -2665,7 +2665,7 @@
       <c r="A42" s="78" t="s">
         <v>59</v>
       </c>
-      <c r="B42" s="174"/>
+      <c r="B42" s="163"/>
       <c r="C42" s="106">
         <v>5000</v>
       </c>
@@ -2695,7 +2695,7 @@
       <c r="A46" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B46" s="175" t="s">
+      <c r="B46" s="164" t="s">
         <v>66</v>
       </c>
       <c r="C46" s="28">
@@ -2711,7 +2711,7 @@
       <c r="A47" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B47" s="176"/>
+      <c r="B47" s="165"/>
       <c r="C47" s="29">
         <v>10</v>
       </c>
@@ -2725,7 +2725,7 @@
       <c r="A48" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B48" s="176"/>
+      <c r="B48" s="165"/>
       <c r="C48" s="29">
         <v>0</v>
       </c>
@@ -2737,7 +2737,7 @@
       <c r="A49" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B49" s="176" t="s">
+      <c r="B49" s="165" t="s">
         <v>68</v>
       </c>
       <c r="C49" s="29">
@@ -2751,7 +2751,7 @@
       <c r="A50" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B50" s="176"/>
+      <c r="B50" s="165"/>
       <c r="C50" s="29">
         <v>10</v>
       </c>
@@ -2763,7 +2763,7 @@
       <c r="A51" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B51" s="176"/>
+      <c r="B51" s="165"/>
       <c r="C51" s="29">
         <v>1</v>
       </c>
@@ -2775,7 +2775,7 @@
       <c r="A52" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B52" s="176" t="s">
+      <c r="B52" s="165" t="s">
         <v>67</v>
       </c>
       <c r="C52" s="29">
@@ -2789,7 +2789,7 @@
       <c r="A53" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B53" s="176"/>
+      <c r="B53" s="165"/>
       <c r="C53" s="29">
         <v>15</v>
       </c>
@@ -2801,7 +2801,7 @@
       <c r="A54" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B54" s="176"/>
+      <c r="B54" s="165"/>
       <c r="C54" s="29">
         <v>2</v>
       </c>
@@ -2813,7 +2813,7 @@
       <c r="A55" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B55" s="173" t="s">
+      <c r="B55" s="161" t="s">
         <v>69</v>
       </c>
       <c r="C55" s="29">
@@ -2827,7 +2827,7 @@
       <c r="A56" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B56" s="173"/>
+      <c r="B56" s="161"/>
       <c r="C56" s="29">
         <v>30</v>
       </c>
@@ -2839,7 +2839,7 @@
       <c r="A57" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B57" s="173"/>
+      <c r="B57" s="161"/>
       <c r="C57" s="29">
         <v>1</v>
       </c>
@@ -2851,7 +2851,7 @@
       <c r="A58" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B58" s="173" t="s">
+      <c r="B58" s="161" t="s">
         <v>83</v>
       </c>
       <c r="C58" s="29">
@@ -2865,7 +2865,7 @@
       <c r="A59" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B59" s="173"/>
+      <c r="B59" s="161"/>
       <c r="C59" s="29">
         <v>150</v>
       </c>
@@ -2877,7 +2877,7 @@
       <c r="A60" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B60" s="173"/>
+      <c r="B60" s="161"/>
       <c r="C60" s="29">
         <v>0</v>
       </c>
@@ -2901,18 +2901,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="A30:A33"/>
     <mergeCell ref="B58:B60"/>
     <mergeCell ref="B40:B42"/>
     <mergeCell ref="B46:B48"/>
     <mergeCell ref="B49:B51"/>
     <mergeCell ref="B52:B54"/>
     <mergeCell ref="B55:B57"/>
-    <mergeCell ref="A4:A8"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="A30:A33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -8673,8 +8673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A43DBB10-3E6D-464B-A3CE-124915F968B4}">
   <dimension ref="A1:Y271"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="75" workbookViewId="0">
+      <selection activeCell="F138" sqref="F138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13658,14 +13658,20 @@
         <v>49</v>
       </c>
       <c r="C137" s="29">
-        <v>0</v>
-      </c>
-      <c r="D137" s="29"/>
+        <v>1</v>
+      </c>
+      <c r="D137" s="29" t="s">
+        <v>107</v>
+      </c>
       <c r="E137" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="F137" s="29"/>
-      <c r="G137" s="39"/>
+        <v>119</v>
+      </c>
+      <c r="F137" s="29">
+        <v>2</v>
+      </c>
+      <c r="G137" s="39" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" s="13"/>
@@ -13868,14 +13874,20 @@
         <v>49</v>
       </c>
       <c r="C151" s="29">
-        <v>0</v>
-      </c>
-      <c r="D151" s="29"/>
+        <v>1</v>
+      </c>
+      <c r="D151" s="29" t="s">
+        <v>107</v>
+      </c>
       <c r="E151" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="F151" s="29"/>
-      <c r="G151" s="39"/>
+        <v>119</v>
+      </c>
+      <c r="F151" s="29">
+        <v>2</v>
+      </c>
+      <c r="G151" s="39" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152" s="13"/>
@@ -14828,6 +14840,24 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="E263:F263"/>
+    <mergeCell ref="K263:L263"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="E249:F249"/>
+    <mergeCell ref="K249:L249"/>
+    <mergeCell ref="E161:F161"/>
+    <mergeCell ref="E175:F175"/>
+    <mergeCell ref="K119:L119"/>
+    <mergeCell ref="Q119:R119"/>
+    <mergeCell ref="E133:F133"/>
+    <mergeCell ref="E147:F147"/>
     <mergeCell ref="W21:X21"/>
     <mergeCell ref="E207:F207"/>
     <mergeCell ref="K207:L207"/>
@@ -14844,24 +14874,6 @@
     <mergeCell ref="E105:F105"/>
     <mergeCell ref="K105:L105"/>
     <mergeCell ref="E119:F119"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="E249:F249"/>
-    <mergeCell ref="K249:L249"/>
-    <mergeCell ref="E161:F161"/>
-    <mergeCell ref="E175:F175"/>
-    <mergeCell ref="K119:L119"/>
-    <mergeCell ref="Q119:R119"/>
-    <mergeCell ref="E133:F133"/>
-    <mergeCell ref="E147:F147"/>
-    <mergeCell ref="E263:F263"/>
-    <mergeCell ref="K263:L263"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="K7:L7"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q22:Q29 W22:W29 E208:E215 E162:E169 K208:K215 E8:E15 K8:K15 Q8:Q15 E176:E183 K250:K255 K257 E250:E257 E264:E271 K264:K271 E22:E29 K22:K29 E36:E43 K36:K43 E50:E57 K50:K57 E64:E71 K64:K71 Q64:Q71 Q78:Q85 E78:E85 K78:K85 K92:K99 E92:E99 K106:K113 E106:E113 K120:K127 E120:E127 Q120:Q127 E134:E141 E148:E155" xr:uid="{504019C3-7A7F-9F49-8A88-D2CEC545D45D}">

</xml_diff>